<commit_message>
adding support for chained processes
</commit_message>
<xml_diff>
--- a/examples/v5/spreadsheet/v5_spleen_plainHeaders.xlsx
+++ b/examples/v5/spreadsheet/v5_spleen_plainHeaders.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/Science/data/pilot_spleen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tburdett/Projects/HumanCellAtlas/ingest-core/examples/v5/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25640" yWindow="0" windowWidth="25560" windowHeight="28800" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="3240" yWindow="460" windowWidth="25560" windowHeight="16640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="protocol" sheetId="17" r:id="rId10"/>
     <sheet name="sequence_file" sheetId="18" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -331,9 +331,6 @@
   </si>
   <si>
     <t>medical_history.treatment</t>
-  </si>
-  <si>
-    <t>genus_species</t>
   </si>
   <si>
     <t>organism_age</t>
@@ -1263,6 +1260,9 @@
   </si>
   <si>
     <t>adult</t>
+  </si>
+  <si>
+    <t>genus_species.text</t>
   </si>
 </sst>
 </file>
@@ -1770,16 +1770,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -1808,25 +1808,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" t="s">
         <v>271</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>272</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>273</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>274</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>275</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>276</v>
-      </c>
-      <c r="G1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1834,66 +1834,66 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>279</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="7" t="s">
         <v>366</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="G5" s="7" t="s">
         <v>370</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -1905,7 +1905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -1923,31 +1923,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B1" t="s">
         <v>287</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>288</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>289</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>290</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>291</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>292</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>293</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>294</v>
-      </c>
-      <c r="I1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1955,7 +1955,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1969,271 +1969,271 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>373</v>
-      </c>
       <c r="D4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -2325,80 +2325,80 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>313</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>318</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>315</v>
-      </c>
       <c r="F5" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>313</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>320</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>315</v>
-      </c>
       <c r="F6" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>313</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -2410,8 +2410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2680,105 +2680,105 @@
         <v>97</v>
       </c>
       <c r="X3" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>322</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>323</v>
       </c>
       <c r="D4" s="4">
         <v>9606</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="U4" s="4" t="s">
         <v>326</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>327</v>
       </c>
       <c r="X4" s="4" t="s">
         <v>73</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Z4" s="4" t="s">
         <v>74</v>
       </c>
       <c r="AA4" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AB4" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="AE4" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="AE4" s="4" t="s">
+      <c r="AF4" t="s">
         <v>330</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>331</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>332</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="AI4" s="8" t="s">
+      <c r="AJ4" t="s">
         <v>334</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>335</v>
       </c>
       <c r="AK4" s="9"/>
     </row>
@@ -2792,7 +2792,7 @@
   <dimension ref="A1:AC9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AC10" sqref="AC10"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2861,52 +2861,52 @@
         <v>59</v>
       </c>
       <c r="L1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" t="s">
         <v>112</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>113</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>114</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>116</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>117</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>118</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>119</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>120</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>121</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>122</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>123</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>124</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>125</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>126</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>127</v>
       </c>
       <c r="AC1" t="s">
         <v>72</v>
@@ -2927,11 +2927,11 @@
         <v>73</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -2947,7 +2947,7 @@
         <v>5</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
@@ -2985,93 +2985,93 @@
         <v>84</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>98</v>
+        <v>401</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AB3" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="AC3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>338</v>
       </c>
       <c r="D4" s="4">
         <v>9606</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="T4" s="4">
         <v>7200</v>
@@ -3080,39 +3080,39 @@
         <v>19800</v>
       </c>
       <c r="AC4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>344</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>345</v>
       </c>
       <c r="D5" s="4">
         <v>9606</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="T5" s="4">
         <v>43200</v>
@@ -3121,39 +3121,39 @@
         <v>54300</v>
       </c>
       <c r="AC5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>347</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>348</v>
       </c>
       <c r="D6" s="4">
         <v>9606</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="T6" s="4">
         <v>86400</v>
@@ -3162,39 +3162,39 @@
         <v>97200</v>
       </c>
       <c r="AC6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>350</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>351</v>
       </c>
       <c r="D7" s="4">
         <v>9606</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="T7" s="4">
         <v>259200</v>
@@ -3203,7 +3203,7 @@
         <v>269100</v>
       </c>
       <c r="AC7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -3220,7 +3220,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView topLeftCell="T3" workbookViewId="0">
-      <selection activeCell="T4" sqref="A4:XFD7"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3282,46 +3282,46 @@
         <v>45</v>
       </c>
       <c r="K1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" t="s">
         <v>146</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>147</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>148</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>149</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>150</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>151</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>152</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>153</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>154</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>155</v>
-      </c>
-      <c r="U1" t="s">
-        <v>156</v>
       </c>
       <c r="V1" t="s">
         <v>59</v>
       </c>
       <c r="W1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X1" t="s">
         <v>157</v>
-      </c>
-      <c r="X1" t="s">
-        <v>158</v>
       </c>
       <c r="Y1" t="s">
         <v>72</v>
@@ -3346,16 +3346,16 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>73</v>
@@ -3396,63 +3396,63 @@
         <v>84</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="X3" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="Y3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D4" s="4">
         <v>9606</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="V4" s="4" t="s">
         <v>73</v>
@@ -3464,16 +3464,16 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D5" s="4">
         <v>9606</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>73</v>
@@ -3485,16 +3485,16 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D6" s="4">
         <v>9606</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="V6" s="4" t="s">
         <v>73</v>
@@ -3506,16 +3506,16 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D7" s="4">
         <v>9606</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="V7" s="4" t="s">
         <v>73</v>
@@ -3553,34 +3553,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" t="s">
         <v>176</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>178</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>179</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I1" t="s">
         <v>181</v>
       </c>
-      <c r="G1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H1" t="s">
-        <v>196</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>182</v>
-      </c>
-      <c r="J1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3588,13 +3588,13 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -3603,51 +3603,51 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B4" t="s">
         <v>397</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
         <v>398</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>399</v>
       </c>
-      <c r="H4" t="s">
-        <v>400</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -3679,40 +3679,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" t="s">
         <v>176</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>178</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>179</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" t="s">
+        <v>201</v>
+      </c>
+      <c r="K1" t="s">
         <v>181</v>
       </c>
-      <c r="G1" t="s">
-        <v>199</v>
-      </c>
-      <c r="H1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I1" t="s">
-        <v>201</v>
-      </c>
-      <c r="J1" t="s">
-        <v>202</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>182</v>
-      </c>
-      <c r="L1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -3720,19 +3720,19 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="G2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -3741,57 +3741,57 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G4" t="s">
+        <v>361</v>
+      </c>
+      <c r="H4" t="s">
         <v>362</v>
       </c>
-      <c r="H4" t="s">
-        <v>363</v>
-      </c>
       <c r="L4" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -3844,115 +3844,115 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" t="s">
         <v>176</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>178</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>179</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K1" t="s">
+        <v>212</v>
+      </c>
+      <c r="L1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N1" t="s">
+        <v>215</v>
+      </c>
+      <c r="O1" t="s">
+        <v>216</v>
+      </c>
+      <c r="P1" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>218</v>
+      </c>
+      <c r="R1" t="s">
+        <v>214</v>
+      </c>
+      <c r="S1" t="s">
+        <v>215</v>
+      </c>
+      <c r="T1" t="s">
+        <v>216</v>
+      </c>
+      <c r="U1" t="s">
+        <v>217</v>
+      </c>
+      <c r="V1" t="s">
+        <v>218</v>
+      </c>
+      <c r="W1" t="s">
+        <v>219</v>
+      </c>
+      <c r="X1" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>221</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>216</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>217</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>181</v>
       </c>
-      <c r="G1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I1" t="s">
-        <v>211</v>
-      </c>
-      <c r="J1" t="s">
-        <v>212</v>
-      </c>
-      <c r="K1" t="s">
-        <v>213</v>
-      </c>
-      <c r="L1" t="s">
-        <v>214</v>
-      </c>
-      <c r="M1" t="s">
-        <v>215</v>
-      </c>
-      <c r="N1" t="s">
-        <v>216</v>
-      </c>
-      <c r="O1" t="s">
-        <v>217</v>
-      </c>
-      <c r="P1" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>219</v>
-      </c>
-      <c r="R1" t="s">
-        <v>215</v>
-      </c>
-      <c r="S1" t="s">
-        <v>216</v>
-      </c>
-      <c r="T1" t="s">
-        <v>217</v>
-      </c>
-      <c r="U1" t="s">
-        <v>218</v>
-      </c>
-      <c r="V1" t="s">
-        <v>219</v>
-      </c>
-      <c r="W1" t="s">
-        <v>220</v>
-      </c>
-      <c r="X1" t="s">
-        <v>221</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>215</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>216</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>217</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>218</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>219</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>209</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>210</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>211</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>212</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>182</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
@@ -3960,13 +3960,13 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -3974,59 +3974,59 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Z2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
@@ -4038,123 +4038,123 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -4163,19 +4163,19 @@
         <v>16</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="W4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="Y4" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AF4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AG4">
         <v>16</v>
@@ -4184,7 +4184,7 @@
         <v>10</v>
       </c>
       <c r="AK4" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -4218,40 +4218,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" t="s">
         <v>176</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>178</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>179</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J1" t="s">
+        <v>263</v>
+      </c>
+      <c r="K1" t="s">
         <v>181</v>
       </c>
-      <c r="G1" t="s">
-        <v>261</v>
-      </c>
-      <c r="H1" t="s">
-        <v>262</v>
-      </c>
-      <c r="I1" t="s">
-        <v>263</v>
-      </c>
-      <c r="J1" t="s">
-        <v>264</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>182</v>
-      </c>
-      <c r="L1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -4259,20 +4259,20 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4280,57 +4280,57 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>388</v>
+      </c>
+      <c r="B4" t="s">
         <v>389</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
+        <v>264</v>
+      </c>
+      <c r="I4" t="s">
+        <v>265</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>390</v>
-      </c>
-      <c r="G4" t="s">
-        <v>265</v>
-      </c>
-      <c r="I4" t="s">
-        <v>266</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>